<commit_message>
Ajout conversion digit to config WS7219+ maj
</commit_message>
<xml_diff>
--- a/MAX7219/matrix_8x8_patterns.xlsx
+++ b/MAX7219/matrix_8x8_patterns.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="51">
   <si>
     <t xml:space="preserve">C7</t>
   </si>
@@ -526,7 +526,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>65</xdr:col>
-      <xdr:colOff>119160</xdr:colOff>
+      <xdr:colOff>119520</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>69480</xdr:rowOff>
     </xdr:from>
@@ -534,7 +534,7 @@
       <xdr:col>89</xdr:col>
       <xdr:colOff>59400</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -547,8 +547,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11799720" y="3690720"/>
-          <a:ext cx="4253400" cy="4115520"/>
+          <a:off x="11800080" y="3690720"/>
+          <a:ext cx="4253040" cy="4115160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -570,8 +570,8 @@
   </sheetPr>
   <dimension ref="B1:AX322"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD30" activeCellId="0" sqref="AD30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2134,7 +2134,7 @@
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
     </sheetView>
   </sheetViews>
@@ -2351,7 +2351,7 @@
   </sheetPr>
   <dimension ref="D1:BO28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -3016,15 +3016,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D1:CF69"/>
+  <dimension ref="D1:DD95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BE53" activeCellId="0" sqref="BE53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CC50" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="DA71" activeCellId="0" sqref="DA71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="1" style="0" width="2.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="0" width="6.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="101" style="0" width="2.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5536,6 +5538,629 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CL78" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM78" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="CN78" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="CO78" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="CP78" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="CQ78" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="CR78" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CS78" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CJ79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="CK79" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="CL79" s="6"/>
+      <c r="CM79" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="CN79" s="7"/>
+      <c r="CO79" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="CP79" s="7"/>
+      <c r="CQ79" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="CR79" s="7"/>
+      <c r="CS79" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="CV79" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="CW79" s="0" t="n">
+        <f aca="false">IF(CL79="x",128,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CX79" s="0" t="n">
+        <f aca="false">IF(CM79="x",128,0)</f>
+        <v>128</v>
+      </c>
+      <c r="CY79" s="0" t="n">
+        <f aca="false">IF(CN79="x",128,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CZ79" s="0" t="n">
+        <f aca="false">IF(CO79="x",128,0)</f>
+        <v>128</v>
+      </c>
+      <c r="DA79" s="0" t="n">
+        <f aca="false">IF(CP79="x",128,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DB79" s="0" t="n">
+        <f aca="false">IF(CQ79="x",128,0)</f>
+        <v>128</v>
+      </c>
+      <c r="DC79" s="0" t="n">
+        <f aca="false">IF(CR79="x",128,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DD79" s="0" t="n">
+        <f aca="false">IF(CS79="x",128,0)</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CJ80" s="1"/>
+      <c r="CK80" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="CL80" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="CM80" s="14"/>
+      <c r="CN80" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CO80" s="14"/>
+      <c r="CP80" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CQ80" s="14"/>
+      <c r="CR80" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CS80" s="15"/>
+      <c r="CV80" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="CW80" s="0" t="n">
+        <f aca="false">IF(CL80="x",64,0)</f>
+        <v>64</v>
+      </c>
+      <c r="CX80" s="0" t="n">
+        <f aca="false">IF(CM80="x",64,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CY80" s="0" t="n">
+        <f aca="false">IF(CN80="x",64,0)</f>
+        <v>64</v>
+      </c>
+      <c r="CZ80" s="0" t="n">
+        <f aca="false">IF(CO80="x",64,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DA80" s="0" t="n">
+        <f aca="false">IF(CP80="x",64,0)</f>
+        <v>64</v>
+      </c>
+      <c r="DB80" s="0" t="n">
+        <f aca="false">IF(CQ80="x",64,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DC80" s="0" t="n">
+        <f aca="false">IF(CR80="x",64,0)</f>
+        <v>64</v>
+      </c>
+      <c r="DD80" s="0" t="n">
+        <f aca="false">IF(CS80="x",64,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CJ81" s="1"/>
+      <c r="CK81" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="CL81" s="13"/>
+      <c r="CM81" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CN81" s="14"/>
+      <c r="CO81" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CP81" s="14"/>
+      <c r="CQ81" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CR81" s="14"/>
+      <c r="CS81" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="CV81" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="CW81" s="0" t="n">
+        <f aca="false">IF(CL81="x",32,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CX81" s="0" t="n">
+        <f aca="false">IF(CM81="x",32,0)</f>
+        <v>32</v>
+      </c>
+      <c r="CY81" s="0" t="n">
+        <f aca="false">IF(CN81="x",32,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CZ81" s="0" t="n">
+        <f aca="false">IF(CO81="x",32,0)</f>
+        <v>32</v>
+      </c>
+      <c r="DA81" s="0" t="n">
+        <f aca="false">IF(CP81="x",32,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DB81" s="0" t="n">
+        <f aca="false">IF(CQ81="x",32,0)</f>
+        <v>32</v>
+      </c>
+      <c r="DC81" s="0" t="n">
+        <f aca="false">IF(CR81="x",32,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DD81" s="0" t="n">
+        <f aca="false">IF(CS81="x",32,0)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CJ82" s="1"/>
+      <c r="CK82" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="CL82" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="CM82" s="14"/>
+      <c r="CN82" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CO82" s="14"/>
+      <c r="CP82" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CQ82" s="14"/>
+      <c r="CR82" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CS82" s="15"/>
+      <c r="CV82" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="CW82" s="0" t="n">
+        <f aca="false">IF(CL82="x",16,0)</f>
+        <v>16</v>
+      </c>
+      <c r="CX82" s="0" t="n">
+        <f aca="false">IF(CM82="x",16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CY82" s="0" t="n">
+        <f aca="false">IF(CN82="x",16,0)</f>
+        <v>16</v>
+      </c>
+      <c r="CZ82" s="0" t="n">
+        <f aca="false">IF(CO82="x",16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DA82" s="0" t="n">
+        <f aca="false">IF(CP82="x",16,0)</f>
+        <v>16</v>
+      </c>
+      <c r="DB82" s="0" t="n">
+        <f aca="false">IF(CQ82="x",16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DC82" s="0" t="n">
+        <f aca="false">IF(CR82="x",16,0)</f>
+        <v>16</v>
+      </c>
+      <c r="DD82" s="0" t="n">
+        <f aca="false">IF(CS82="x",16,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CJ83" s="1"/>
+      <c r="CK83" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="CL83" s="13"/>
+      <c r="CM83" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CN83" s="14"/>
+      <c r="CO83" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CP83" s="14"/>
+      <c r="CQ83" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CR83" s="14"/>
+      <c r="CS83" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="CV83" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="CW83" s="0" t="n">
+        <f aca="false">IF(CL83="x",8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CX83" s="0" t="n">
+        <f aca="false">IF(CM83="x",8,0)</f>
+        <v>8</v>
+      </c>
+      <c r="CY83" s="0" t="n">
+        <f aca="false">IF(CN83="x",8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CZ83" s="0" t="n">
+        <f aca="false">IF(CO83="x",8,0)</f>
+        <v>8</v>
+      </c>
+      <c r="DA83" s="0" t="n">
+        <f aca="false">IF(CP83="x",8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DB83" s="0" t="n">
+        <f aca="false">IF(CQ83="x",8,0)</f>
+        <v>8</v>
+      </c>
+      <c r="DC83" s="0" t="n">
+        <f aca="false">IF(CR83="x",8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DD83" s="0" t="n">
+        <f aca="false">IF(CS83="x",8,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CJ84" s="1"/>
+      <c r="CK84" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="CL84" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="CM84" s="14"/>
+      <c r="CN84" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CO84" s="14"/>
+      <c r="CP84" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CQ84" s="14"/>
+      <c r="CR84" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CS84" s="15"/>
+      <c r="CV84" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="CW84" s="0" t="n">
+        <f aca="false">IF(CL84="x",4,0)</f>
+        <v>4</v>
+      </c>
+      <c r="CX84" s="0" t="n">
+        <f aca="false">IF(CM84="x",4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CY84" s="0" t="n">
+        <f aca="false">IF(CN84="x",4,0)</f>
+        <v>4</v>
+      </c>
+      <c r="CZ84" s="0" t="n">
+        <f aca="false">IF(CO84="x",4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DA84" s="0" t="n">
+        <f aca="false">IF(CP84="x",4,0)</f>
+        <v>4</v>
+      </c>
+      <c r="DB84" s="0" t="n">
+        <f aca="false">IF(CQ84="x",4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DC84" s="0" t="n">
+        <f aca="false">IF(CR84="x",4,0)</f>
+        <v>4</v>
+      </c>
+      <c r="DD84" s="0" t="n">
+        <f aca="false">IF(CS84="x",4,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CJ85" s="1"/>
+      <c r="CK85" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="CL85" s="13"/>
+      <c r="CM85" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CN85" s="14"/>
+      <c r="CO85" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CP85" s="14"/>
+      <c r="CQ85" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="CR85" s="14"/>
+      <c r="CS85" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="CV85" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="CW85" s="0" t="n">
+        <f aca="false">IF(CL85="x",2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CX85" s="0" t="n">
+        <f aca="false">IF(CM85="x",2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="CY85" s="0" t="n">
+        <f aca="false">IF(CN85="x",2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CZ85" s="0" t="n">
+        <f aca="false">IF(CO85="x",2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="DA85" s="0" t="n">
+        <f aca="false">IF(CP85="x",2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DB85" s="0" t="n">
+        <f aca="false">IF(CQ85="x",2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="DC85" s="0" t="n">
+        <f aca="false">IF(CR85="x",2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DD85" s="0" t="n">
+        <f aca="false">IF(CS85="x",2,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CJ86" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="CK86" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="CL86" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="CM86" s="21"/>
+      <c r="CN86" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="CO86" s="21"/>
+      <c r="CP86" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="CQ86" s="21"/>
+      <c r="CR86" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="CS86" s="22"/>
+      <c r="CV86" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="CW86" s="0" t="n">
+        <f aca="false">IF(CL86="x",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="CX86" s="0" t="n">
+        <f aca="false">IF(CM86="x",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="CY86" s="0" t="n">
+        <f aca="false">IF(CN86="x",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="CZ86" s="0" t="n">
+        <f aca="false">IF(CO86="x",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DA86" s="0" t="n">
+        <f aca="false">IF(CP86="x",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="DB86" s="0" t="n">
+        <f aca="false">IF(CQ86="x",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="DC86" s="0" t="n">
+        <f aca="false">IF(CR86="x",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="DD86" s="0" t="n">
+        <f aca="false">IF(CS86="x",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CV88" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="CW88" s="26" t="str">
+        <f aca="false">DEC2HEX((SUM(CW79:CW86)),2)</f>
+        <v>55</v>
+      </c>
+      <c r="CX88" s="26"/>
+      <c r="CY88" s="26"/>
+      <c r="CZ88" s="26"/>
+      <c r="DA88" s="26"/>
+      <c r="DB88" s="26"/>
+      <c r="DC88" s="26"/>
+      <c r="DD88" s="26"/>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CV89" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="CW89" s="26"/>
+      <c r="CX89" s="26" t="str">
+        <f aca="false">DEC2HEX(SUM(CX79:CX86),2)</f>
+        <v>AA</v>
+      </c>
+      <c r="CY89" s="26"/>
+      <c r="CZ89" s="26"/>
+      <c r="DA89" s="26"/>
+      <c r="DB89" s="26"/>
+      <c r="DC89" s="26"/>
+      <c r="DD89" s="26"/>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CV90" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="CW90" s="26"/>
+      <c r="CX90" s="26"/>
+      <c r="CY90" s="26" t="str">
+        <f aca="false">DEC2HEX(SUM(CY79:CY86),2)</f>
+        <v>55</v>
+      </c>
+      <c r="CZ90" s="26"/>
+      <c r="DA90" s="26"/>
+      <c r="DB90" s="26"/>
+      <c r="DC90" s="26"/>
+      <c r="DD90" s="26"/>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CV91" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="CW91" s="26"/>
+      <c r="CX91" s="26"/>
+      <c r="CY91" s="26"/>
+      <c r="CZ91" s="26" t="str">
+        <f aca="false">DEC2HEX(SUM(CZ79:CZ86),2)</f>
+        <v>AA</v>
+      </c>
+      <c r="DA91" s="26"/>
+      <c r="DB91" s="26"/>
+      <c r="DC91" s="26"/>
+      <c r="DD91" s="26"/>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CV92" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="CW92" s="26"/>
+      <c r="CX92" s="26"/>
+      <c r="CY92" s="26"/>
+      <c r="CZ92" s="26"/>
+      <c r="DA92" s="26" t="str">
+        <f aca="false">DEC2HEX(SUM(DA79:DA86),2)</f>
+        <v>55</v>
+      </c>
+      <c r="DB92" s="26"/>
+      <c r="DC92" s="26"/>
+      <c r="DD92" s="26"/>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CV93" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="CW93" s="26"/>
+      <c r="CX93" s="26"/>
+      <c r="CY93" s="26"/>
+      <c r="CZ93" s="26"/>
+      <c r="DA93" s="26"/>
+      <c r="DB93" s="26" t="str">
+        <f aca="false">DEC2HEX(SUM(DB79:DB86),2)</f>
+        <v>AA</v>
+      </c>
+      <c r="DC93" s="26"/>
+      <c r="DD93" s="26"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CV94" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="CW94" s="26"/>
+      <c r="CX94" s="26"/>
+      <c r="CY94" s="26"/>
+      <c r="CZ94" s="26"/>
+      <c r="DA94" s="26"/>
+      <c r="DB94" s="26"/>
+      <c r="DC94" s="26" t="str">
+        <f aca="false">DEC2HEX(SUM(DC79:DC86),2)</f>
+        <v>55</v>
+      </c>
+      <c r="DD94" s="26"/>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CV95" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="CW95" s="26"/>
+      <c r="CX95" s="26"/>
+      <c r="CY95" s="26"/>
+      <c r="CZ95" s="26"/>
+      <c r="DA95" s="26"/>
+      <c r="DB95" s="26"/>
+      <c r="DC95" s="26"/>
+      <c r="DD95" s="26" t="str">
+        <f aca="false">DEC2HEX(SUM(DD79:DD86),2)</f>
+        <v>AA</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="D1:K1"/>

</xml_diff>